<commit_message>
Update section_schedules.xlsx: Modify schedule data to reflect recent changes in academic structure and improve data accuracy.
</commit_message>
<xml_diff>
--- a/public/templates/section_schedules.xlsx
+++ b/public/templates/section_schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daust\dev\lapontificia\pontiapp-laravel\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\dev\pontiapp-laravel\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88CF712-C596-4D3D-BDA1-3CAC898B66B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B72D83-3C97-4C20-9488-82AB2C937A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{140B157C-7BA0-4AAF-9127-20F3E698D59F}"/>
+    <workbookView xWindow="4185" yWindow="2475" windowWidth="21600" windowHeight="11295" xr2:uid="{140B157C-7BA0-4AAF-9127-20F3E698D59F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
     <t>Docente</t>
   </si>
   <si>
-    <t>&lt;</t>
+    <t>Periodo</t>
   </si>
 </sst>
 </file>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -509,10 +509,10 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>

</xml_diff>

<commit_message>
Update section_schedules.xlsx: Replace existing schedule data with the latest version to ensure accuracy and reflect current academic information.
</commit_message>
<xml_diff>
--- a/public/templates/section_schedules.xlsx
+++ b/public/templates/section_schedules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\dev\pontiapp-laravel\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B72D83-3C97-4C20-9488-82AB2C937A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1674C25-E0ED-4DC0-9BA0-1612AA94B6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="2475" windowWidth="21600" windowHeight="11295" xr2:uid="{140B157C-7BA0-4AAF-9127-20F3E698D59F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{140B157C-7BA0-4AAF-9127-20F3E698D59F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Sección</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Periodo</t>
+  </si>
+  <si>
+    <t>Docente Correo</t>
   </si>
 </sst>
 </file>
@@ -160,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -172,6 +175,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,7 +194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -506,13 +510,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1971CC-AAD9-4F5E-9C5F-A21B0C6B0DBC}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
@@ -530,10 +534,11 @@
     <col min="14" max="14" width="17.28515625" style="3" customWidth="1"/>
     <col min="15" max="15" width="37.85546875" style="3" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="3"/>
+    <col min="17" max="17" width="23.140625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -581,6 +586,9 @@
       </c>
       <c r="P1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update section_schedules.xlsx with the latest schedule data to ensure accuracy and reflect current academic information.
</commit_message>
<xml_diff>
--- a/public/templates/section_schedules.xlsx
+++ b/public/templates/section_schedules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\dev\pontiapp-laravel\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1674C25-E0ED-4DC0-9BA0-1612AA94B6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B7720E-6708-4E1F-85D3-95302DF63177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{140B157C-7BA0-4AAF-9127-20F3E698D59F}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +109,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -163,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -176,6 +184,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,7 +203,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,22 +519,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1971CC-AAD9-4F5E-9C5F-A21B0C6B0DBC}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="37" style="3" customWidth="1"/>
+    <col min="8" max="8" width="43.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="3" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="3" customWidth="1"/>
@@ -533,8 +542,8 @@
     <col min="13" max="13" width="8.85546875" style="3" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" style="3" customWidth="1"/>
     <col min="15" max="15" width="37.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="23.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="36.28515625" style="3" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -591,6 +600,9 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>